<commit_message>
Enable file upload in ChatKitPanel with support for images and PDFs
</commit_message>
<xml_diff>
--- a/mcp/Quote_Formic_Acid_2025-10-27.xlsx
+++ b/mcp/Quote_Formic_Acid_2025-10-27.xlsx
@@ -1028,7 +1028,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Formic acid, 85%</t>
+          <t>Formic Acid extrapure AR, 98%</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1043,37 +1043,41 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>ASF2569</t>
+          <t>Part A</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>100 ml bottle</t>
+          <t>500 ml</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>220.0</v>
+        <v>500.0</v>
       </c>
       <c r="H15" t="n">
         <v>0.18</v>
       </c>
-      <c r="I15" t="n">
-        <v>180.4</v>
+      <c r="I15">
+        <f>G15*(1-H15)</f>
+        <v>410.00000000000006</v>
       </c>
       <c r="J15" t="n">
         <v>1</v>
       </c>
-      <c r="K15" t="n">
-        <v>180.4</v>
+      <c r="K15">
+        <f>I15*J15</f>
+        <v>410.00000000000006</v>
       </c>
       <c r="L15" t="n">
         <v>0.18</v>
       </c>
-      <c r="M15" t="n">
-        <v>32.472</v>
-      </c>
-      <c r="N15" t="n">
-        <v>212.872</v>
+      <c r="M15">
+        <f>K15*L15</f>
+        <v>73.80000000000001</v>
+      </c>
+      <c r="N15">
+        <f>K15+M15</f>
+        <v>483.80000000000007</v>
       </c>
     </row>
     <row r="16">
@@ -1097,37 +1101,41 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>ASF2569</t>
+          <t>Consumable</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>500 ml bottle</t>
+          <t>100 ml</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>407.0</v>
+        <v>220.0</v>
       </c>
       <c r="H16" t="n">
         <v>0.18</v>
       </c>
-      <c r="I16" t="n">
-        <v>333.74</v>
+      <c r="I16">
+        <f>G16*(1-H16)</f>
+        <v>180.4</v>
       </c>
       <c r="J16" t="n">
         <v>1</v>
       </c>
-      <c r="K16" t="n">
-        <v>333.74</v>
+      <c r="K16">
+        <f>I16*J16</f>
+        <v>180.4</v>
       </c>
       <c r="L16" t="n">
         <v>0.18</v>
       </c>
-      <c r="M16" t="n">
-        <v>60.0732</v>
-      </c>
-      <c r="N16" t="n">
-        <v>393.8132</v>
+      <c r="M16">
+        <f>K16*L16</f>
+        <v>32.472</v>
+      </c>
+      <c r="N16">
+        <f>K16+M16</f>
+        <v>212.872</v>
       </c>
     </row>
     <row r="17">
@@ -1151,37 +1159,41 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>ASF2569</t>
+          <t>Consumable</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2.5 L can</t>
+          <t>500 ml</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>1320.0</v>
+        <v>407.0</v>
       </c>
       <c r="H17" t="n">
         <v>0.18</v>
       </c>
-      <c r="I17" t="n">
-        <v>1082.4</v>
+      <c r="I17">
+        <f>G17*(1-H17)</f>
+        <v>333.74</v>
       </c>
       <c r="J17" t="n">
         <v>1</v>
       </c>
-      <c r="K17" t="n">
-        <v>1082.4</v>
+      <c r="K17">
+        <f>I17*J17</f>
+        <v>333.74</v>
       </c>
       <c r="L17" t="n">
         <v>0.18</v>
       </c>
-      <c r="M17" t="n">
-        <v>194.83200000000002</v>
-      </c>
-      <c r="N17" t="n">
-        <v>1277.2320000000002</v>
+      <c r="M17">
+        <f>K17*L17</f>
+        <v>60.0732</v>
+      </c>
+      <c r="N17">
+        <f>K17+M17</f>
+        <v>393.8132</v>
       </c>
     </row>
     <row r="18">
@@ -1190,7 +1202,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Formic acid, 98%</t>
+          <t>Formic acid, 85%</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1205,37 +1217,41 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>ASF1362</t>
+          <t>Consumable</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>500 ml bottle</t>
+          <t>2.5 L</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>770.0</v>
+        <v>1320.0</v>
       </c>
       <c r="H18" t="n">
         <v>0.18</v>
       </c>
-      <c r="I18" t="n">
-        <v>631.4000000000001</v>
+      <c r="I18">
+        <f>G18*(1-H18)</f>
+        <v>1082.4</v>
       </c>
       <c r="J18" t="n">
         <v>1</v>
       </c>
-      <c r="K18" t="n">
-        <v>631.4000000000001</v>
+      <c r="K18">
+        <f>I18*J18</f>
+        <v>1082.4</v>
       </c>
       <c r="L18" t="n">
         <v>0.18</v>
       </c>
-      <c r="M18" t="n">
-        <v>113.65200000000002</v>
-      </c>
-      <c r="N18" t="n">
-        <v>745.0520000000001</v>
+      <c r="M18">
+        <f>K18*L18</f>
+        <v>194.83200000000002</v>
+      </c>
+      <c r="N18">
+        <f>K18+M18</f>
+        <v>1277.2320000000002</v>
       </c>
     </row>
     <row r="19">
@@ -1259,37 +1275,41 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>ASF1362</t>
+          <t>Consumable</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2.5 L can</t>
+          <t>500 ml</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>3220.0</v>
+        <v>770.0</v>
       </c>
       <c r="H19" t="n">
         <v>0.18</v>
       </c>
-      <c r="I19" t="n">
-        <v>2640.4</v>
+      <c r="I19">
+        <f>G19*(1-H19)</f>
+        <v>631.4000000000001</v>
       </c>
       <c r="J19" t="n">
         <v>1</v>
       </c>
-      <c r="K19" t="n">
-        <v>2640.4</v>
+      <c r="K19">
+        <f>I19*J19</f>
+        <v>631.4000000000001</v>
       </c>
       <c r="L19" t="n">
         <v>0.18</v>
       </c>
-      <c r="M19" t="n">
-        <v>475.272</v>
-      </c>
-      <c r="N19" t="n">
-        <v>3115.672</v>
+      <c r="M19">
+        <f>K19*L19</f>
+        <v>113.65200000000002</v>
+      </c>
+      <c r="N19">
+        <f>K19+M19</f>
+        <v>745.0520000000001</v>
       </c>
     </row>
     <row r="20">
@@ -1298,7 +1318,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Formic acid</t>
+          <t>Formic acid, 98%</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1313,37 +1333,41 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>ALF1072</t>
+          <t>Consumable</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>500 ml bottle</t>
+          <t>2.5 L</t>
         </is>
       </c>
       <c r="G20" t="n">
-        <v>770.0</v>
+        <v>3220.0</v>
       </c>
       <c r="H20" t="n">
         <v>0.18</v>
       </c>
-      <c r="I20" t="n">
-        <v>631.4000000000001</v>
+      <c r="I20">
+        <f>G20*(1-H20)</f>
+        <v>2640.4</v>
       </c>
       <c r="J20" t="n">
         <v>1</v>
       </c>
-      <c r="K20" t="n">
-        <v>631.4000000000001</v>
+      <c r="K20">
+        <f>I20*J20</f>
+        <v>2640.4</v>
       </c>
       <c r="L20" t="n">
         <v>0.18</v>
       </c>
-      <c r="M20" t="n">
-        <v>113.65200000000002</v>
-      </c>
-      <c r="N20" t="n">
-        <v>745.0520000000001</v>
+      <c r="M20">
+        <f>K20*L20</f>
+        <v>475.272</v>
+      </c>
+      <c r="N20">
+        <f>K20+M20</f>
+        <v>3115.672</v>
       </c>
     </row>
     <row r="21">
@@ -1367,64 +1391,111 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>ALF1072</t>
+          <t>Consumable</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2.5 L can</t>
+          <t>500 ml</t>
         </is>
       </c>
       <c r="G21" t="n">
-        <v>3080.0</v>
+        <v>770.0</v>
       </c>
       <c r="H21" t="n">
         <v>0.18</v>
       </c>
-      <c r="I21" t="n">
-        <v>2525.6000000000004</v>
+      <c r="I21">
+        <f>G21*(1-H21)</f>
+        <v>631.4000000000001</v>
       </c>
       <c r="J21" t="n">
         <v>1</v>
       </c>
-      <c r="K21" t="n">
-        <v>2525.6000000000004</v>
+      <c r="K21">
+        <f>I21*J21</f>
+        <v>631.4000000000001</v>
       </c>
       <c r="L21" t="n">
         <v>0.18</v>
       </c>
-      <c r="M21" t="n">
+      <c r="M21">
+        <f>K21*L21</f>
+        <v>113.65200000000002</v>
+      </c>
+      <c r="N21">
+        <f>K21+M21</f>
+        <v>745.0520000000001</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>8</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Formic acid</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>64-18-6</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>29151100</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Consumable</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2.5 L</t>
+        </is>
+      </c>
+      <c r="G22" t="n">
+        <v>3080.0</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="I22">
+        <f>G22*(1-H22)</f>
+        <v>2525.6000000000004</v>
+      </c>
+      <c r="J22" t="n">
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <f>I22*J22</f>
+        <v>2525.6000000000004</v>
+      </c>
+      <c r="L22" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="M22">
+        <f>K22*L22</f>
         <v>454.60800000000006</v>
       </c>
-      <c r="N21" t="n">
+      <c r="N22">
+        <f>K22+M22</f>
         <v>2980.2080000000005</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
+    <row r="23">
+      <c r="A23" t="inlineStr">
         <is>
           <t>TOTAL</t>
         </is>
       </c>
-      <c r="N22" t="n">
-        <v>9469.9</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="41"/>
-      <c r="B23" s="42"/>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="41"/>
-      <c r="G23" s="43"/>
-      <c r="H23" s="41"/>
-      <c r="I23" s="43"/>
-      <c r="J23" s="41"/>
-      <c r="K23" s="43"/>
-      <c r="L23" s="42"/>
-      <c r="M23" s="44"/>
-      <c r="N23" s="45"/>
+      <c r="N23">
+        <f>SUM(N15:N22)</f>
+        <v>9953.7</v>
+      </c>
     </row>
     <row r="24" spans="1:14" ns2:dyDescent="0.3">
       <c r="A24" s="41"/>
@@ -1444,16 +1515,12 @@
     </row>
     <row r="24">
       <c r="A24" s="41"/>
-      <c r="B24" s="42" t="s">
-        <v>54</v>
-      </c>
+      <c r="B24" s="42"/>
       <c r="C24" s="41"/>
       <c r="D24" s="41"/>
       <c r="E24" s="41"/>
       <c r="F24" s="41"/>
-      <c r="G24" s="43" t="s">
-        <v>56</v>
-      </c>
+      <c r="G24" s="43"/>
       <c r="H24" s="41"/>
       <c r="I24" s="43"/>
       <c r="J24" s="41"/>
@@ -1485,14 +1552,14 @@
     <row r="25">
       <c r="A25" s="41"/>
       <c r="B25" s="42" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C25" s="41"/>
       <c r="D25" s="41"/>
       <c r="E25" s="41"/>
       <c r="F25" s="41"/>
       <c r="G25" s="43" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H25" s="41"/>
       <c r="I25" s="43"/>
@@ -1524,12 +1591,16 @@
     </row>
     <row r="26">
       <c r="A26" s="41"/>
-      <c r="B26" s="42"/>
+      <c r="B26" s="42" t="s">
+        <v>55</v>
+      </c>
       <c r="C26" s="41"/>
       <c r="D26" s="41"/>
       <c r="E26" s="41"/>
       <c r="F26" s="41"/>
-      <c r="G26" s="43"/>
+      <c r="G26" s="43" t="s">
+        <v>57</v>
+      </c>
       <c r="H26" s="41"/>
       <c r="I26" s="43"/>
       <c r="J26" s="41"/>
@@ -1555,12 +1626,20 @@
       <c r="N27" s="45"/>
     </row>
     <row r="27">
-      <c r="A27" s="1"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="H27" s="2"/>
+      <c r="A27" s="41"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="41"/>
+      <c r="F27" s="41"/>
+      <c r="G27" s="43"/>
+      <c r="H27" s="41"/>
+      <c r="I27" s="43"/>
+      <c r="J27" s="41"/>
+      <c r="K27" s="43"/>
+      <c r="L27" s="42"/>
+      <c r="M27" s="44"/>
+      <c r="N27" s="45"/>
     </row>
     <row r="28" spans="1:14" ns2:dyDescent="0.3">
       <c r="A28" s="1"/>
@@ -1571,12 +1650,9 @@
       <c r="H28" s="2"/>
     </row>
     <row r="28">
-      <c r="A28" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="B28" s="17"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
+      <c r="A28" s="1"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="H28" s="2"/>
@@ -1593,8 +1669,8 @@
       <c r="H29" s="2"/>
     </row>
     <row r="29">
-      <c r="A29" s="16" t="s">
-        <v>44</v>
+      <c r="A29" s="36" t="s">
+        <v>43</v>
       </c>
       <c r="B29" s="17"/>
       <c r="C29" s="18"/>
@@ -1616,7 +1692,7 @@
     </row>
     <row r="30">
       <c r="A30" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B30" s="17"/>
       <c r="C30" s="18"/>
@@ -1638,7 +1714,7 @@
     </row>
     <row r="31">
       <c r="A31" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B31" s="17"/>
       <c r="C31" s="18"/>
@@ -1660,7 +1736,7 @@
     </row>
     <row r="32">
       <c r="A32" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B32" s="17"/>
       <c r="C32" s="18"/>
@@ -1681,7 +1757,9 @@
       <c r="H33" s="2"/>
     </row>
     <row r="33">
-      <c r="A33" s="16"/>
+      <c r="A33" s="16" t="s">
+        <v>47</v>
+      </c>
       <c r="B33" s="17"/>
       <c r="C33" s="18"/>
       <c r="D33" s="18"/>
@@ -1699,12 +1777,10 @@
       <c r="H34" s="2"/>
     </row>
     <row r="34">
-      <c r="A34" s="37" t="s">
-        <v>48</v>
-      </c>
-      <c r="B34" s="37"/>
-      <c r="C34" s="38"/>
-      <c r="D34" s="38"/>
+      <c r="A34" s="16"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="H34" s="2"/>
@@ -1721,7 +1797,9 @@
       <c r="H35" s="2"/>
     </row>
     <row r="35">
-      <c r="A35" s="37"/>
+      <c r="A35" s="37" t="s">
+        <v>48</v>
+      </c>
       <c r="B35" s="37"/>
       <c r="C35" s="38"/>
       <c r="D35" s="38"/>
@@ -1739,9 +1817,7 @@
       <c r="H36" s="2"/>
     </row>
     <row r="36">
-      <c r="A36" s="37" t="s">
-        <v>49</v>
-      </c>
+      <c r="A36" s="37"/>
       <c r="B36" s="37"/>
       <c r="C36" s="38"/>
       <c r="D36" s="38"/>
@@ -1761,7 +1837,9 @@
       <c r="H37" s="2"/>
     </row>
     <row r="37">
-      <c r="A37" s="37"/>
+      <c r="A37" s="37" t="s">
+        <v>49</v>
+      </c>
       <c r="B37" s="37"/>
       <c r="C37" s="38"/>
       <c r="D37" s="38"/>
@@ -1779,9 +1857,7 @@
       <c r="H38" s="2"/>
     </row>
     <row r="38">
-      <c r="A38" s="37" t="s">
-        <v>50</v>
-      </c>
+      <c r="A38" s="37"/>
       <c r="B38" s="37"/>
       <c r="C38" s="38"/>
       <c r="D38" s="38"/>
@@ -1801,7 +1877,9 @@
       <c r="H39" s="2"/>
     </row>
     <row r="39">
-      <c r="A39" s="37"/>
+      <c r="A39" s="37" t="s">
+        <v>50</v>
+      </c>
       <c r="B39" s="37"/>
       <c r="C39" s="38"/>
       <c r="D39" s="38"/>
@@ -1819,8 +1897,8 @@
       <c r="H40" s="2"/>
     </row>
     <row r="40">
-      <c r="A40" s="39"/>
-      <c r="B40" s="39"/>
+      <c r="A40" s="37"/>
+      <c r="B40" s="37"/>
       <c r="C40" s="38"/>
       <c r="D40" s="38"/>
       <c r="E40" s="2"/>
@@ -1837,8 +1915,8 @@
       <c r="H41" s="2"/>
     </row>
     <row r="41">
-      <c r="A41" s="37"/>
-      <c r="B41" s="37"/>
+      <c r="A41" s="39"/>
+      <c r="B41" s="39"/>
       <c r="C41" s="38"/>
       <c r="D41" s="38"/>
       <c r="E41" s="2"/>
@@ -1855,10 +1933,8 @@
       <c r="H42" s="2"/>
     </row>
     <row r="42">
-      <c r="A42" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="B42" s="40"/>
+      <c r="A42" s="37"/>
+      <c r="B42" s="37"/>
       <c r="C42" s="38"/>
       <c r="D42" s="38"/>
       <c r="E42" s="2"/>
@@ -1866,6 +1942,17 @@
       <c r="H42" s="2"/>
     </row>
     <row r="43" spans="1:8" ns2:dyDescent="0.3">
+      <c r="A43" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="B43" s="40"/>
+      <c r="C43" s="38"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="H43" s="2"/>
+    </row>
+    <row r="43">
       <c r="A43" s="37" t="s">
         <v>51</v>
       </c>

</xml_diff>